<commit_message>
Version 1 simulated annealing
</commit_message>
<xml_diff>
--- a/tp5-busquedas-locales/code/hill_climbing_results.xlsx
+++ b/tp5-busquedas-locales/code/hill_climbing_results.xlsx
@@ -455,10 +455,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.0009970664978027344</v>
       </c>
     </row>
     <row r="3">
@@ -466,10 +466,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0009968280792236328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -499,10 +499,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.0009970664978027344</v>
       </c>
     </row>
     <row r="7">
@@ -521,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -532,10 +532,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.0009982585906982422</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +543,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0009973049163818359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -609,10 +609,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0009970664978027344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -620,7 +620,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -664,10 +664,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0009975433349609375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -686,10 +686,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.0009973049163818359</v>
       </c>
     </row>
     <row r="24">
@@ -697,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -708,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -719,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0009975433349609375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -741,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.0009970664978027344</v>
       </c>
     </row>
     <row r="29">
@@ -752,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -774,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>8</v>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C32" t="n">
-        <v>0.002991676330566406</v>
+        <v>0.01501989364624023</v>
       </c>
     </row>
     <row r="33">
@@ -796,10 +796,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="n">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C33" t="n">
-        <v>0.03490805625915527</v>
+        <v>0.05096960067749023</v>
       </c>
     </row>
     <row r="34">
@@ -807,10 +807,10 @@
         <v>8</v>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01096987724304199</v>
+        <v>0.004053115844726562</v>
       </c>
     </row>
     <row r="35">
@@ -818,10 +818,10 @@
         <v>8</v>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C35" t="n">
-        <v>0.001994609832763672</v>
+        <v>0.003989458084106445</v>
       </c>
     </row>
     <row r="36">
@@ -829,10 +829,10 @@
         <v>8</v>
       </c>
       <c r="B36" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C36" t="n">
-        <v>0.005983829498291016</v>
+        <v>0.01499509811401367</v>
       </c>
     </row>
     <row r="37">
@@ -840,10 +840,10 @@
         <v>8</v>
       </c>
       <c r="B37" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="C37" t="n">
-        <v>0.03191471099853516</v>
+        <v>0.0109708309173584</v>
       </c>
     </row>
     <row r="38">
@@ -854,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>0.002991914749145508</v>
+        <v>0.002991676330566406</v>
       </c>
     </row>
     <row r="39">
@@ -862,10 +862,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="n">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03690099716186523</v>
+        <v>0.01598763465881348</v>
       </c>
     </row>
     <row r="40">
@@ -873,10 +873,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C40" t="n">
-        <v>0.003989458084106445</v>
+        <v>0.0210258960723877</v>
       </c>
     </row>
     <row r="41">
@@ -884,10 +884,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C41" t="n">
-        <v>0.004986763000488281</v>
+        <v>0.01723527908325195</v>
       </c>
     </row>
     <row r="42">
@@ -895,10 +895,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="n">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>0.06781840324401855</v>
+        <v>0.007978916168212891</v>
       </c>
     </row>
     <row r="43">
@@ -906,10 +906,10 @@
         <v>8</v>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C43" t="n">
-        <v>0.002992153167724609</v>
+        <v>0.003988981246948242</v>
       </c>
     </row>
     <row r="44">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C44" t="n">
-        <v>0.002992391586303711</v>
+        <v>0.004986763000488281</v>
       </c>
     </row>
     <row r="45">
@@ -928,10 +928,10 @@
         <v>8</v>
       </c>
       <c r="B45" t="n">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="C45" t="n">
-        <v>0.009972810745239258</v>
+        <v>0.05186128616333008</v>
       </c>
     </row>
     <row r="46">
@@ -939,10 +939,10 @@
         <v>8</v>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C46" t="n">
-        <v>0.003989458084106445</v>
+        <v>0.05994772911071777</v>
       </c>
     </row>
     <row r="47">
@@ -950,10 +950,10 @@
         <v>8</v>
       </c>
       <c r="B47" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C47" t="n">
-        <v>0.003989458084106445</v>
+        <v>0.009034633636474609</v>
       </c>
     </row>
     <row r="48">
@@ -961,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.001994609832763672</v>
+        <v>0.003048181533813477</v>
       </c>
     </row>
     <row r="49">
@@ -972,10 +972,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="n">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01994657516479492</v>
+        <v>0.05893468856811523</v>
       </c>
     </row>
     <row r="50">
@@ -983,10 +983,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>0.004986763000488281</v>
+        <v>0.002992153167724609</v>
       </c>
     </row>
     <row r="51">
@@ -994,10 +994,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C51" t="n">
-        <v>0.005984067916870117</v>
+        <v>0.003989219665527344</v>
       </c>
     </row>
     <row r="52">
@@ -1005,10 +1005,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="n">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C52" t="n">
-        <v>0.007978677749633789</v>
+        <v>0.06302213668823242</v>
       </c>
     </row>
     <row r="53">
@@ -1016,10 +1016,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="n">
-        <v>164</v>
+        <v>9</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1077117919921875</v>
+        <v>0.004987001419067383</v>
       </c>
     </row>
     <row r="54">
@@ -1027,10 +1027,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0359039306640625</v>
+        <v>0.0160679817199707</v>
       </c>
     </row>
     <row r="55">
@@ -1038,10 +1038,10 @@
         <v>8</v>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C55" t="n">
-        <v>0.002992153167724609</v>
+        <v>0.02298641204833984</v>
       </c>
     </row>
     <row r="56">
@@ -1049,10 +1049,10 @@
         <v>8</v>
       </c>
       <c r="B56" t="n">
-        <v>1000</v>
+        <v>6</v>
       </c>
       <c r="C56" t="n">
-        <v>0.6592371463775635</v>
+        <v>0.003989934921264648</v>
       </c>
     </row>
     <row r="57">
@@ -1060,10 +1060,10 @@
         <v>8</v>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C57" t="n">
-        <v>0.002992153167724609</v>
+        <v>0.01296520233154297</v>
       </c>
     </row>
     <row r="58">
@@ -1071,10 +1071,10 @@
         <v>8</v>
       </c>
       <c r="B58" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01296544075012207</v>
+        <v>0.01102709770202637</v>
       </c>
     </row>
     <row r="59">
@@ -1082,10 +1082,10 @@
         <v>8</v>
       </c>
       <c r="B59" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C59" t="n">
-        <v>0.01196789741516113</v>
+        <v>0.005984067916870117</v>
       </c>
     </row>
     <row r="60">
@@ -1093,10 +1093,10 @@
         <v>8</v>
       </c>
       <c r="B60" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>0.007978439331054688</v>
+        <v>0.002042770385742188</v>
       </c>
     </row>
     <row r="61">
@@ -1104,10 +1104,10 @@
         <v>8</v>
       </c>
       <c r="B61" t="n">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="C61" t="n">
-        <v>0.06382966041564941</v>
+        <v>0.008975982666015625</v>
       </c>
     </row>
     <row r="62">
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="B62" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C62" t="n">
-        <v>0.02393579483032227</v>
+        <v>0.009973287582397461</v>
       </c>
     </row>
     <row r="63">
@@ -1126,10 +1126,10 @@
         <v>10</v>
       </c>
       <c r="B63" t="n">
-        <v>35</v>
+        <v>211</v>
       </c>
       <c r="C63" t="n">
-        <v>0.05485320091247559</v>
+        <v>0.3339748382568359</v>
       </c>
     </row>
     <row r="64">
@@ -1137,10 +1137,10 @@
         <v>10</v>
       </c>
       <c r="B64" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C64" t="n">
-        <v>0.008976221084594727</v>
+        <v>0.07803630828857422</v>
       </c>
     </row>
     <row r="65">
@@ -1148,10 +1148,10 @@
         <v>10</v>
       </c>
       <c r="B65" t="n">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.01296496391296387</v>
+        <v>0.1043069362640381</v>
       </c>
     </row>
     <row r="66">
@@ -1159,10 +1159,10 @@
         <v>10</v>
       </c>
       <c r="B66" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C66" t="n">
-        <v>0.005984067916870117</v>
+        <v>0.06881594657897949</v>
       </c>
     </row>
     <row r="67">
@@ -1170,10 +1170,10 @@
         <v>10</v>
       </c>
       <c r="B67" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0219414234161377</v>
+        <v>0.09188389778137207</v>
       </c>
     </row>
     <row r="68">
@@ -1181,10 +1181,10 @@
         <v>10</v>
       </c>
       <c r="B68" t="n">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2074456214904785</v>
+        <v>0.0110161304473877</v>
       </c>
     </row>
     <row r="69">
@@ -1192,10 +1192,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C69" t="n">
-        <v>0.02094388008117676</v>
+        <v>0.01199579238891602</v>
       </c>
     </row>
     <row r="70">
@@ -1203,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C70" t="n">
-        <v>0.04188823699951172</v>
+        <v>0.03898525238037109</v>
       </c>
     </row>
     <row r="71">
@@ -1214,10 +1214,10 @@
         <v>10</v>
       </c>
       <c r="B71" t="n">
-        <v>107</v>
+        <v>1000</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1675515174865723</v>
+        <v>1.586769819259644</v>
       </c>
     </row>
     <row r="72">
@@ -1225,10 +1225,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="n">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C72" t="n">
-        <v>0.08577060699462891</v>
+        <v>0.04288530349731445</v>
       </c>
     </row>
     <row r="73">
@@ -1236,10 +1236,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1874988079071045</v>
+        <v>0.1924850940704346</v>
       </c>
     </row>
     <row r="74">
@@ -1247,10 +1247,10 @@
         <v>10</v>
       </c>
       <c r="B74" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C74" t="n">
-        <v>0.02593064308166504</v>
+        <v>0.01795220375061035</v>
       </c>
     </row>
     <row r="75">
@@ -1258,10 +1258,10 @@
         <v>10</v>
       </c>
       <c r="B75" t="n">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1914877891540527</v>
+        <v>0.01795244216918945</v>
       </c>
     </row>
     <row r="76">
@@ -1269,10 +1269,10 @@
         <v>10</v>
       </c>
       <c r="B76" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C76" t="n">
-        <v>0.007978916168212891</v>
+        <v>0.04088973999023438</v>
       </c>
     </row>
     <row r="77">
@@ -1280,10 +1280,10 @@
         <v>10</v>
       </c>
       <c r="B77" t="n">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C77" t="n">
-        <v>0.01595711708068848</v>
+        <v>0.1146936416625977</v>
       </c>
     </row>
     <row r="78">
@@ -1291,10 +1291,10 @@
         <v>10</v>
       </c>
       <c r="B78" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C78" t="n">
-        <v>0.02293896675109863</v>
+        <v>0.01994681358337402</v>
       </c>
     </row>
     <row r="79">
@@ -1302,10 +1302,10 @@
         <v>10</v>
       </c>
       <c r="B79" t="n">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0468745231628418</v>
+        <v>0.08676767349243164</v>
       </c>
     </row>
     <row r="80">
@@ -1313,10 +1313,10 @@
         <v>10</v>
       </c>
       <c r="B80" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0468745231628418</v>
+        <v>0.03291201591491699</v>
       </c>
     </row>
     <row r="81">
@@ -1324,10 +1324,10 @@
         <v>10</v>
       </c>
       <c r="B81" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C81" t="n">
-        <v>0.01196837425231934</v>
+        <v>0.08178138732910156</v>
       </c>
     </row>
     <row r="82">
@@ -1335,10 +1335,10 @@
         <v>10</v>
       </c>
       <c r="B82" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C82" t="n">
-        <v>0.01296520233154297</v>
+        <v>0.008975982666015625</v>
       </c>
     </row>
     <row r="83">
@@ -1346,10 +1346,10 @@
         <v>10</v>
       </c>
       <c r="B83" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C83" t="n">
-        <v>0.01894927024841309</v>
+        <v>0.01695466041564941</v>
       </c>
     </row>
     <row r="84">
@@ -1357,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="B84" t="n">
-        <v>36</v>
+        <v>234</v>
       </c>
       <c r="C84" t="n">
-        <v>0.05585050582885742</v>
+        <v>0.3650243282318115</v>
       </c>
     </row>
     <row r="85">
@@ -1368,10 +1368,10 @@
         <v>10</v>
       </c>
       <c r="B85" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C85" t="n">
-        <v>0.02992010116577148</v>
+        <v>0.01296520233154297</v>
       </c>
     </row>
     <row r="86">
@@ -1379,10 +1379,10 @@
         <v>10</v>
       </c>
       <c r="B86" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C86" t="n">
-        <v>0.008976221084594727</v>
+        <v>0.06682133674621582</v>
       </c>
     </row>
     <row r="87">
@@ -1390,10 +1390,10 @@
         <v>10</v>
       </c>
       <c r="B87" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C87" t="n">
-        <v>0.01595711708068848</v>
+        <v>0.02293848991394043</v>
       </c>
     </row>
     <row r="88">
@@ -1401,10 +1401,10 @@
         <v>10</v>
       </c>
       <c r="B88" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C88" t="n">
-        <v>0.183509349822998</v>
+        <v>0.1565811634063721</v>
       </c>
     </row>
     <row r="89">
@@ -1412,10 +1412,10 @@
         <v>10</v>
       </c>
       <c r="B89" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C89" t="n">
-        <v>0.02094388008117676</v>
+        <v>0.01296567916870117</v>
       </c>
     </row>
     <row r="90">
@@ -1423,10 +1423,10 @@
         <v>10</v>
       </c>
       <c r="B90" t="n">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1625652313232422</v>
+        <v>0.009973049163818359</v>
       </c>
     </row>
     <row r="91">
@@ -1434,10 +1434,10 @@
         <v>10</v>
       </c>
       <c r="B91" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0608375072479248</v>
+        <v>0.03390932083129883</v>
       </c>
     </row>
     <row r="92">
@@ -1445,10 +1445,10 @@
         <v>12</v>
       </c>
       <c r="B92" t="n">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C92" t="n">
-        <v>0.2767982482910156</v>
+        <v>0.1117012500762939</v>
       </c>
     </row>
     <row r="93">
@@ -1456,10 +1456,10 @@
         <v>12</v>
       </c>
       <c r="B93" t="n">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1077120304107666</v>
+        <v>0.2054505348205566</v>
       </c>
     </row>
     <row r="94">
@@ -1467,10 +1467,10 @@
         <v>12</v>
       </c>
       <c r="B94" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1934826374053955</v>
+        <v>0.05684828758239746</v>
       </c>
     </row>
     <row r="95">
@@ -1478,10 +1478,10 @@
         <v>12</v>
       </c>
       <c r="B95" t="n">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="C95" t="n">
-        <v>0.341087818145752</v>
+        <v>0.05385637283325195</v>
       </c>
     </row>
     <row r="96">
@@ -1489,10 +1489,10 @@
         <v>12</v>
       </c>
       <c r="B96" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1077871322631836</v>
+        <v>0.1894927024841309</v>
       </c>
     </row>
     <row r="97">
@@ -1500,10 +1500,10 @@
         <v>12</v>
       </c>
       <c r="B97" t="n">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="C97" t="n">
-        <v>0.2130532264709473</v>
+        <v>0.04089069366455078</v>
       </c>
     </row>
     <row r="98">
@@ -1511,10 +1511,10 @@
         <v>12</v>
       </c>
       <c r="B98" t="n">
-        <v>13</v>
+        <v>288</v>
       </c>
       <c r="C98" t="n">
-        <v>0.04094123840332031</v>
+        <v>0.9255251884460449</v>
       </c>
     </row>
     <row r="99">
@@ -1522,10 +1522,10 @@
         <v>12</v>
       </c>
       <c r="B99" t="n">
-        <v>45</v>
+        <v>1000</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1438090801239014</v>
+        <v>3.311326742172241</v>
       </c>
     </row>
     <row r="100">
@@ -1533,10 +1533,10 @@
         <v>12</v>
       </c>
       <c r="B100" t="n">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="C100" t="n">
-        <v>0.3592171669006348</v>
+        <v>0.1186830997467041</v>
       </c>
     </row>
     <row r="101">
@@ -1544,10 +1544,10 @@
         <v>12</v>
       </c>
       <c r="B101" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C101" t="n">
-        <v>0.06981348991394043</v>
+        <v>0.1815574169158936</v>
       </c>
     </row>
     <row r="102">
@@ -1555,10 +1555,10 @@
         <v>12</v>
       </c>
       <c r="B102" t="n">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C102" t="n">
-        <v>0.01994681358337402</v>
+        <v>0.3426620960235596</v>
       </c>
     </row>
     <row r="103">
@@ -1566,10 +1566,10 @@
         <v>12</v>
       </c>
       <c r="B103" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1077117919921875</v>
+        <v>0.077362060546875</v>
       </c>
     </row>
     <row r="104">
@@ -1577,10 +1577,10 @@
         <v>12</v>
       </c>
       <c r="B104" t="n">
-        <v>47</v>
+        <v>1000</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1511049270629883</v>
+        <v>3.26144814491272</v>
       </c>
     </row>
     <row r="105">
@@ -1588,10 +1588,10 @@
         <v>12</v>
       </c>
       <c r="B105" t="n">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="C105" t="n">
-        <v>0.3111639022827148</v>
+        <v>0.1132400035858154</v>
       </c>
     </row>
     <row r="106">
@@ -1599,10 +1599,10 @@
         <v>12</v>
       </c>
       <c r="B106" t="n">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="C106" t="n">
-        <v>0.3321402072906494</v>
+        <v>0.09229373931884766</v>
       </c>
     </row>
     <row r="107">
@@ -1610,10 +1610,10 @@
         <v>12</v>
       </c>
       <c r="B107" t="n">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="C107" t="n">
-        <v>0.07679486274719238</v>
+        <v>0.5266921520233154</v>
       </c>
     </row>
     <row r="108">
@@ -1621,10 +1621,10 @@
         <v>12</v>
       </c>
       <c r="B108" t="n">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="C108" t="n">
-        <v>0.2647969722747803</v>
+        <v>0.03789877891540527</v>
       </c>
     </row>
     <row r="109">
@@ -1632,10 +1632,10 @@
         <v>12</v>
       </c>
       <c r="B109" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C109" t="n">
-        <v>0.04787206649780273</v>
+        <v>0.01795196533203125</v>
       </c>
     </row>
     <row r="110">
@@ -1643,10 +1643,10 @@
         <v>12</v>
       </c>
       <c r="B110" t="n">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1740396022796631</v>
+        <v>0.02349543571472168</v>
       </c>
     </row>
     <row r="111">
@@ -1654,10 +1654,10 @@
         <v>12</v>
       </c>
       <c r="B111" t="n">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C111" t="n">
-        <v>0.04488015174865723</v>
+        <v>0.1595730781555176</v>
       </c>
     </row>
     <row r="112">
@@ -1665,10 +1665,10 @@
         <v>12</v>
       </c>
       <c r="B112" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C112" t="n">
-        <v>0.02792501449584961</v>
+        <v>0.163118839263916</v>
       </c>
     </row>
     <row r="113">
@@ -1676,10 +1676,10 @@
         <v>12</v>
       </c>
       <c r="B113" t="n">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="C113" t="n">
-        <v>0.03490662574768066</v>
+        <v>0.4109954833984375</v>
       </c>
     </row>
     <row r="114">
@@ -1687,10 +1687,10 @@
         <v>12</v>
       </c>
       <c r="B114" t="n">
-        <v>1000</v>
+        <v>14</v>
       </c>
       <c r="C114" t="n">
-        <v>3.167116641998291</v>
+        <v>0.04388236999511719</v>
       </c>
     </row>
     <row r="115">
@@ -1698,10 +1698,10 @@
         <v>12</v>
       </c>
       <c r="B115" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1870050430297852</v>
+        <v>0.05738091468811035</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>86</v>
       </c>
       <c r="C116" t="n">
-        <v>0.2732794284820557</v>
+        <v>0.2698144912719727</v>
       </c>
     </row>
     <row r="117">
@@ -1720,10 +1720,10 @@
         <v>12</v>
       </c>
       <c r="B117" t="n">
-        <v>176</v>
+        <v>69</v>
       </c>
       <c r="C117" t="n">
-        <v>0.556018590927124</v>
+        <v>0.2179520130157471</v>
       </c>
     </row>
     <row r="118">
@@ -1731,10 +1731,10 @@
         <v>12</v>
       </c>
       <c r="B118" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C118" t="n">
-        <v>0.04388284683227539</v>
+        <v>0.02293872833251953</v>
       </c>
     </row>
     <row r="119">
@@ -1742,10 +1742,10 @@
         <v>12</v>
       </c>
       <c r="B119" t="n">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C119" t="n">
-        <v>0.235370397567749</v>
+        <v>0.04288554191589355</v>
       </c>
     </row>
     <row r="120">
@@ -1753,10 +1753,10 @@
         <v>12</v>
       </c>
       <c r="B120" t="n">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C120" t="n">
-        <v>0.03191494941711426</v>
+        <v>0.1730988025665283</v>
       </c>
     </row>
     <row r="121">
@@ -1764,10 +1764,10 @@
         <v>12</v>
       </c>
       <c r="B121" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C121" t="n">
-        <v>0.07878923416137695</v>
+        <v>0.04886913299560547</v>
       </c>
     </row>
     <row r="122">
@@ -1775,10 +1775,10 @@
         <v>15</v>
       </c>
       <c r="B122" t="n">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C122" t="n">
-        <v>0.4418184757232666</v>
+        <v>0.09731864929199219</v>
       </c>
     </row>
     <row r="123">
@@ -1786,10 +1786,10 @@
         <v>15</v>
       </c>
       <c r="B123" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C123" t="n">
-        <v>0.04488015174865723</v>
+        <v>0.1700806617736816</v>
       </c>
     </row>
     <row r="124">
@@ -1797,10 +1797,10 @@
         <v>15</v>
       </c>
       <c r="B124" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C124" t="n">
-        <v>0.4408211708068848</v>
+        <v>0.3346431255340576</v>
       </c>
     </row>
     <row r="125">
@@ -1808,10 +1808,10 @@
         <v>15</v>
       </c>
       <c r="B125" t="n">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="C125" t="n">
-        <v>0.2433493137359619</v>
+        <v>0.6964032649993896</v>
       </c>
     </row>
     <row r="126">
@@ -1819,10 +1819,10 @@
         <v>15</v>
       </c>
       <c r="B126" t="n">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1515946388244629</v>
+        <v>0.4014637470245361</v>
       </c>
     </row>
     <row r="127">
@@ -1830,10 +1830,10 @@
         <v>15</v>
       </c>
       <c r="B127" t="n">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C127" t="n">
-        <v>0.09873580932617188</v>
+        <v>0.4813365936279297</v>
       </c>
     </row>
     <row r="128">
@@ -1841,10 +1841,10 @@
         <v>15</v>
       </c>
       <c r="B128" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C128" t="n">
-        <v>0.05285906791687012</v>
+        <v>0.06981348991394043</v>
       </c>
     </row>
     <row r="129">
@@ -1852,10 +1852,10 @@
         <v>15</v>
       </c>
       <c r="B129" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C129" t="n">
-        <v>0.3959410190582275</v>
+        <v>0.4943270683288574</v>
       </c>
     </row>
     <row r="130">
@@ -1863,10 +1863,10 @@
         <v>15</v>
       </c>
       <c r="B130" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1136960983276367</v>
+        <v>0.2433490753173828</v>
       </c>
     </row>
     <row r="131">
@@ -1874,10 +1874,10 @@
         <v>15</v>
       </c>
       <c r="B131" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C131" t="n">
-        <v>0.09075736999511719</v>
+        <v>0.2424540519714355</v>
       </c>
     </row>
     <row r="132">
@@ -1885,10 +1885,10 @@
         <v>15</v>
       </c>
       <c r="B132" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1595730781555176</v>
+        <v>0.3103036880493164</v>
       </c>
     </row>
     <row r="133">
@@ -1896,10 +1896,10 @@
         <v>15</v>
       </c>
       <c r="B133" t="n">
-        <v>386</v>
+        <v>27</v>
       </c>
       <c r="C133" t="n">
-        <v>2.92418098449707</v>
+        <v>0.2079861164093018</v>
       </c>
     </row>
     <row r="134">
@@ -1907,10 +1907,10 @@
         <v>15</v>
       </c>
       <c r="B134" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1585760116577148</v>
+        <v>0.1725387573242188</v>
       </c>
     </row>
     <row r="135">
@@ -1918,10 +1918,10 @@
         <v>15</v>
       </c>
       <c r="B135" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C135" t="n">
-        <v>0.1216747760772705</v>
+        <v>0.1361770629882812</v>
       </c>
     </row>
     <row r="136">
@@ -1929,10 +1929,10 @@
         <v>15</v>
       </c>
       <c r="B136" t="n">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1505973339080811</v>
+        <v>0.5890274047851562</v>
       </c>
     </row>
     <row r="137">
@@ -1940,10 +1940,10 @@
         <v>15</v>
       </c>
       <c r="B137" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1356372833251953</v>
+        <v>0.1651113033294678</v>
       </c>
     </row>
     <row r="138">
@@ -1951,10 +1951,10 @@
         <v>15</v>
       </c>
       <c r="B138" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1057171821594238</v>
+        <v>0.2020139694213867</v>
       </c>
     </row>
     <row r="139">
@@ -1962,10 +1962,10 @@
         <v>15</v>
       </c>
       <c r="B139" t="n">
-        <v>1000</v>
+        <v>23</v>
       </c>
       <c r="C139" t="n">
-        <v>7.626607179641724</v>
+        <v>0.1730706691741943</v>
       </c>
     </row>
     <row r="140">
@@ -1973,10 +1973,10 @@
         <v>15</v>
       </c>
       <c r="B140" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1208961009979248</v>
+        <v>0.2508831024169922</v>
       </c>
     </row>
     <row r="141">
@@ -1984,10 +1984,10 @@
         <v>15</v>
       </c>
       <c r="B141" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C141" t="n">
-        <v>0.2872323989868164</v>
+        <v>0.07579779624938965</v>
       </c>
     </row>
     <row r="142">
@@ -1995,10 +1995,10 @@
         <v>15</v>
       </c>
       <c r="B142" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="C142" t="n">
-        <v>0.6821753978729248</v>
+        <v>0.1062495708465576</v>
       </c>
     </row>
     <row r="143">
@@ -2006,10 +2006,10 @@
         <v>15</v>
       </c>
       <c r="B143" t="n">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="C143" t="n">
-        <v>1.316479921340942</v>
+        <v>0.2678253650665283</v>
       </c>
     </row>
     <row r="144">
@@ -2017,10 +2017,10 @@
         <v>15</v>
       </c>
       <c r="B144" t="n">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1505975723266602</v>
+        <v>0.4788534641265869</v>
       </c>
     </row>
     <row r="145">
@@ -2028,10 +2028,10 @@
         <v>15</v>
       </c>
       <c r="B145" t="n">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="C145" t="n">
-        <v>0.2124316692352295</v>
+        <v>0.9910814762115479</v>
       </c>
     </row>
     <row r="146">
@@ -2039,10 +2039,10 @@
         <v>15</v>
       </c>
       <c r="B146" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C146" t="n">
-        <v>0.09973335266113281</v>
+        <v>0.08533835411071777</v>
       </c>
     </row>
     <row r="147">
@@ -2050,10 +2050,10 @@
         <v>15</v>
       </c>
       <c r="B147" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C147" t="n">
-        <v>0.0608372688293457</v>
+        <v>0.137631893157959</v>
       </c>
     </row>
     <row r="148">
@@ -2061,10 +2061,10 @@
         <v>15</v>
       </c>
       <c r="B148" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C148" t="n">
-        <v>0.2273921966552734</v>
+        <v>0.1501352787017822</v>
       </c>
     </row>
     <row r="149">
@@ -2072,10 +2072,10 @@
         <v>15</v>
       </c>
       <c r="B149" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1934823989868164</v>
+        <v>0.2189524173736572</v>
       </c>
     </row>
     <row r="150">
@@ -2083,10 +2083,10 @@
         <v>15</v>
       </c>
       <c r="B150" t="n">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C150" t="n">
-        <v>0.09175467491149902</v>
+        <v>0.6010074615478516</v>
       </c>
     </row>
     <row r="151">
@@ -2094,10 +2094,10 @@
         <v>15</v>
       </c>
       <c r="B151" t="n">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="C151" t="n">
-        <v>0.4821298122406006</v>
+        <v>0.06981348991394043</v>
       </c>
     </row>
   </sheetData>

</xml_diff>